<commit_message>
removed unnecessary spacing after intro paragraph
</commit_message>
<xml_diff>
--- a/Teaching Data/11-09-2018 Ashford 4th years.xlsx
+++ b/Teaching Data/11-09-2018 Ashford 4th years.xlsx
@@ -1,29 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vig/Data/Programming/WebDev/ECG-teaching-questionnaire/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vig/Data/Programming/WebDev/ECG-teaching-questionnaire/Teaching Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D79F9025-0F26-094C-9C0B-7FD1BCAEA84B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321020DD-1FBC-584E-A942-165E1E23703A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="export 11-09-2018" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v2.0" hidden="1">'export 11-09-2018'!$I$2:$I$5</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">'export 11-09-2018'!$J$1</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">'export 11-09-2018'!$J$2:$J$5</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">'export 11-09-2018'!$K$1</definedName>
-    <definedName name="_xlchart.v2.4" hidden="1">'export 11-09-2018'!$K$2:$K$5</definedName>
-    <definedName name="_xlchart.v2.5" hidden="1">'export 11-09-2018'!$L$1</definedName>
-    <definedName name="_xlchart.v2.6" hidden="1">'export 11-09-2018'!$L$2:$L$5</definedName>
-  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -79,7 +70,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -2851,16 +2842,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>298449</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>158749</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>446616</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>306916</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2887,16 +2878,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>292100</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>317500</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3220,11 +3211,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>